<commit_message>
update unit test init kbn setting test
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/DataInitKbnSetting.xlsx
+++ b/CloudTest/SampleData/DataInitKbnSetting.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="RAIIN_KBN_MST" sheetId="1" r:id="rId1"/>
@@ -395,7 +395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -614,7 +614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix get sheet name
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/DataInitKbnSetting.xlsx
+++ b/CloudTest/SampleData/DataInitKbnSetting.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7D37D9-8222-4878-821E-C525B36F6E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAIIN_KBN_MST" sheetId="1" r:id="rId1"/>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -392,11 +393,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,7 +406,7 @@
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,7 +446,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -611,11 +612,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,22 +678,6 @@
       <c r="I2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I3" s="1"/>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I4" s="1"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I5" s="1"/>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I6" s="1"/>
-      <c r="L6" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update unit test setting
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/DataInitKbnSetting.xlsx
+++ b/CloudTest/SampleData/DataInitKbnSetting.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="RAIIN_KBN_MST" sheetId="1" r:id="rId1"/>
     <sheet name="RAIIN_KBN_DETAIL" sheetId="2" r:id="rId2"/>
     <sheet name="RAIIN_KBN_INF" sheetId="3" r:id="rId3"/>
+    <sheet name="RAIIN_KBN_KOUI" sheetId="4" r:id="rId4"/>
+    <sheet name="KOUI_KBN_MST" sheetId="5" r:id="rId5"/>
+    <sheet name="RAIIN_KBN_ITEM" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>HP_ID</t>
   </si>
@@ -75,6 +78,33 @@
   </si>
   <si>
     <t>SEQ_NO</t>
+  </si>
+  <si>
+    <t>KOUI_KBN_ID</t>
+  </si>
+  <si>
+    <t>KOUI_KBN1</t>
+  </si>
+  <si>
+    <t>KOUI_KBN2</t>
+  </si>
+  <si>
+    <t>KOUI_GRP_NAME</t>
+  </si>
+  <si>
+    <t>KOUI_NAME</t>
+  </si>
+  <si>
+    <t>KOUI_NAME_CHECK</t>
+  </si>
+  <si>
+    <t>KOUI_GRP_NAME_CHECK</t>
+  </si>
+  <si>
+    <t>ITEM_CD</t>
+  </si>
+  <si>
+    <t>IS_EXCLUDE</t>
   </si>
 </sst>
 </file>
@@ -395,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +479,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +645,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,4 +726,193 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>9999</v>
+      </c>
+      <c r="C2">
+        <v>999</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>999</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>999</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>9999</v>
+      </c>
+      <c r="C2">
+        <v>999</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>613120001</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update unit test init kbn
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/DataInitKbnSetting.xlsx
+++ b/CloudTest/SampleData/DataInitKbnSetting.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="RAIIN_KBN_MST" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="RAIIN_KBN_KOUI" sheetId="4" r:id="rId4"/>
     <sheet name="KOUI_KBN_MST" sheetId="5" r:id="rId5"/>
     <sheet name="RAIIN_KBN_ITEM" sheetId="6" r:id="rId6"/>
+    <sheet name="RAIIN_KBN_YOYAKU" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>HP_ID</t>
   </si>
@@ -105,6 +106,9 @@
   </si>
   <si>
     <t>IS_EXCLUDE</t>
+  </si>
+  <si>
+    <t>YOYAKU_CD</t>
   </si>
 </sst>
 </file>
@@ -854,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,4 +919,59 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>9999</v>
+      </c>
+      <c r="C2">
+        <v>999</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>12345</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>